<commit_message>
Add modified: Plan, Check, Cases
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="184">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -571,6 +571,12 @@
   <si>
     <t>Поддерживаются основные жесты при работе с сенсорными экранами (swipe back и т.д.)</t>
   </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
 </sst>
 </file>
 
@@ -954,15 +960,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -972,22 +969,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1002,14 +999,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1085"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1305,7 +1311,7 @@
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="39.75" thickBot="1">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1341,15 +1347,17 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" ht="52.5" thickBot="1">
-      <c r="A2" s="17"/>
+    <row r="2" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A2" s="30"/>
       <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -1373,15 +1381,17 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="52.5" thickBot="1">
-      <c r="A3" s="18"/>
+    <row r="3" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A3" s="31"/>
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -1405,15 +1415,17 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" ht="78" thickBot="1">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A4" s="31"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -1437,15 +1449,17 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A5" s="18"/>
+    <row r="5" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A5" s="31"/>
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1469,15 +1483,17 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" ht="78" thickBot="1">
-      <c r="A6" s="18"/>
+    <row r="6" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A6" s="31"/>
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1501,15 +1517,17 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A7" s="32"/>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="8" t="s">
@@ -1536,10 +1554,10 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1563,8 +1581,8 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" ht="52.5" thickBot="1">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A9" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1573,7 +1591,9 @@
       <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -1597,15 +1617,17 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A10" s="24"/>
+    <row r="10" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A10" s="34"/>
       <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -1629,15 +1651,17 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" ht="255.75" thickBot="1">
-      <c r="A11" s="24"/>
+    <row r="11" spans="1:26" ht="45.75" thickBot="1">
+      <c r="A11" s="34"/>
       <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1661,15 +1685,17 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" ht="231" thickBot="1">
-      <c r="A12" s="24"/>
+    <row r="12" spans="1:26" ht="39.75" thickBot="1">
+      <c r="A12" s="34"/>
       <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="8" t="s">
@@ -1695,15 +1721,17 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26" ht="141.75" thickBot="1">
-      <c r="A13" s="24"/>
+    <row r="13" spans="1:26" ht="27" thickBot="1">
+      <c r="A13" s="34"/>
       <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1727,15 +1755,17 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="141.75" thickBot="1">
-      <c r="A14" s="24"/>
+    <row r="14" spans="1:26" ht="27" thickBot="1">
+      <c r="A14" s="34"/>
       <c r="B14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1759,15 +1789,17 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" ht="103.5" thickBot="1">
-      <c r="A15" s="24"/>
+    <row r="15" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A15" s="34"/>
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1791,15 +1823,17 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26" ht="129" thickBot="1">
-      <c r="A16" s="24"/>
+    <row r="16" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A16" s="34"/>
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1823,15 +1857,17 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A17" s="24"/>
+    <row r="17" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A17" s="34"/>
       <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1855,15 +1891,17 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
-    <row r="18" spans="1:26" ht="39.75" thickBot="1">
-      <c r="A18" s="24"/>
+    <row r="18" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A18" s="34"/>
       <c r="B18" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1887,15 +1925,17 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A19" s="24"/>
+    <row r="19" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A19" s="34"/>
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1919,15 +1959,17 @@
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A20" s="24"/>
+    <row r="20" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A20" s="34"/>
       <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1951,15 +1993,17 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" spans="1:26" ht="52.5" thickBot="1">
-      <c r="A21" s="24"/>
+    <row r="21" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A21" s="34"/>
       <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1983,15 +2027,17 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" spans="1:26" ht="52.5" thickBot="1">
-      <c r="A22" s="24"/>
+    <row r="22" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A22" s="34"/>
       <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -2015,15 +2061,17 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="1:26" ht="231" thickBot="1">
-      <c r="A23" s="24"/>
+    <row r="23" spans="1:26" ht="39.75" thickBot="1">
+      <c r="A23" s="34"/>
       <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="8" t="s">
@@ -2049,15 +2097,17 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="1:26" ht="231" thickBot="1">
-      <c r="A24" s="24"/>
+    <row r="24" spans="1:26" ht="39.75" thickBot="1">
+      <c r="A24" s="34"/>
       <c r="B24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="8" t="s">
@@ -2083,15 +2133,17 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="1:26" ht="195.75" thickBot="1">
-      <c r="A25" s="24"/>
+    <row r="25" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A25" s="34"/>
       <c r="B25" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="8" t="s">
@@ -2117,15 +2169,17 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" spans="1:26" ht="180.75" thickBot="1">
-      <c r="A26" s="24"/>
+    <row r="26" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A26" s="34"/>
       <c r="B26" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="8" t="s">
@@ -2151,15 +2205,17 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
     </row>
-    <row r="27" spans="1:26" ht="285.75" thickBot="1">
-      <c r="A27" s="24"/>
+    <row r="27" spans="1:26" ht="45.75" thickBot="1">
+      <c r="A27" s="34"/>
       <c r="B27" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="8" t="s">
@@ -2185,15 +2241,17 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:26" ht="330.75" thickBot="1">
-      <c r="A28" s="24"/>
+    <row r="28" spans="1:26" ht="45.75" thickBot="1">
+      <c r="A28" s="34"/>
       <c r="B28" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -2217,15 +2275,17 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A29" s="24"/>
+    <row r="29" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A29" s="34"/>
       <c r="B29" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -2249,15 +2309,17 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A30" s="24"/>
+    <row r="30" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A30" s="34"/>
       <c r="B30" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2281,15 +2343,17 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A31" s="25"/>
+    <row r="31" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A31" s="35"/>
       <c r="B31" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="8" t="s">
@@ -2316,9 +2380,9 @@
       <c r="Z31" s="5"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="10"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -2343,8 +2407,8 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A33" s="26" t="s">
+    <row r="33" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A33" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -2353,7 +2417,9 @@
       <c r="C33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -2377,15 +2443,17 @@
       <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="1:26" ht="135.75" thickBot="1">
-      <c r="A34" s="27"/>
+    <row r="34" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A34" s="25"/>
       <c r="B34" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -2409,15 +2477,17 @@
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row r="35" spans="1:26" ht="165.75" thickBot="1">
-      <c r="A35" s="27"/>
+    <row r="35" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A35" s="25"/>
       <c r="B35" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="6"/>
+      <c r="D35" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -2441,15 +2511,17 @@
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A36" s="27"/>
+    <row r="36" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A36" s="25"/>
       <c r="B36" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="6"/>
+      <c r="D36" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -2473,15 +2545,17 @@
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
     </row>
-    <row r="37" spans="1:26" ht="150.75" thickBot="1">
-      <c r="A37" s="27"/>
+    <row r="37" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A37" s="25"/>
       <c r="B37" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="6"/>
+      <c r="D37" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2505,15 +2579,17 @@
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
     </row>
-    <row r="38" spans="1:26" ht="135.75" thickBot="1">
-      <c r="A38" s="28"/>
+    <row r="38" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A38" s="21"/>
       <c r="B38" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="6"/>
+      <c r="D38" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -2538,9 +2614,9 @@
       <c r="Z38" s="5"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A39" s="20"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="10"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -2565,8 +2641,8 @@
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A40" s="26" t="s">
+    <row r="40" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A40" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -2575,7 +2651,9 @@
       <c r="C40" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="6"/>
+      <c r="D40" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -2599,15 +2677,17 @@
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
     </row>
-    <row r="41" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A41" s="27"/>
+    <row r="41" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A41" s="25"/>
       <c r="B41" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="6"/>
+      <c r="D41" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -2631,15 +2711,17 @@
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
     </row>
-    <row r="42" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A42" s="27"/>
+    <row r="42" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A42" s="25"/>
       <c r="B42" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="6"/>
+      <c r="D42" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -2663,15 +2745,17 @@
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
     </row>
-    <row r="43" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A43" s="27"/>
+    <row r="43" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A43" s="25"/>
       <c r="B43" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="6"/>
+      <c r="D43" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -2695,15 +2779,17 @@
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
     </row>
-    <row r="44" spans="1:26" ht="180.75" thickBot="1">
-      <c r="A44" s="27"/>
+    <row r="44" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A44" s="25"/>
       <c r="B44" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="6"/>
+      <c r="D44" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -2727,15 +2813,17 @@
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
     </row>
-    <row r="45" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A45" s="27"/>
+    <row r="45" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A45" s="25"/>
       <c r="B45" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="6"/>
+      <c r="D45" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -2759,15 +2847,17 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
     </row>
-    <row r="46" spans="1:26" ht="65.25" thickBot="1">
-      <c r="A46" s="28"/>
+    <row r="46" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A46" s="21"/>
       <c r="B46" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="6"/>
+      <c r="D46" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -2792,9 +2882,9 @@
       <c r="Z46" s="5"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A47" s="20"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="22"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="10"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -2819,8 +2909,8 @@
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
     </row>
-    <row r="48" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A48" s="26" t="s">
+    <row r="48" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A48" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B48" s="7" t="s">
@@ -2829,7 +2919,9 @@
       <c r="C48" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="6"/>
+      <c r="D48" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -2853,15 +2945,17 @@
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
     </row>
-    <row r="49" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A49" s="27"/>
+    <row r="49" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A49" s="25"/>
       <c r="B49" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D49" s="6"/>
+      <c r="D49" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
@@ -2885,15 +2979,17 @@
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
     </row>
-    <row r="50" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A50" s="27"/>
+    <row r="50" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A50" s="25"/>
       <c r="B50" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="6"/>
+      <c r="D50" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -2917,15 +3013,17 @@
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
     </row>
-    <row r="51" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A51" s="27"/>
+    <row r="51" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A51" s="25"/>
       <c r="B51" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="6"/>
+      <c r="D51" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -2949,15 +3047,17 @@
       <c r="Y51" s="5"/>
       <c r="Z51" s="5"/>
     </row>
-    <row r="52" spans="1:26" ht="165.75" thickBot="1">
-      <c r="A52" s="28"/>
+    <row r="52" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A52" s="21"/>
       <c r="B52" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
@@ -2981,8 +3081,8 @@
       <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
     </row>
-    <row r="53" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A53" s="26" t="s">
+    <row r="53" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A53" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -2991,7 +3091,9 @@
       <c r="C53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="6"/>
+      <c r="D53" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
@@ -3015,15 +3117,17 @@
       <c r="Y53" s="5"/>
       <c r="Z53" s="5"/>
     </row>
-    <row r="54" spans="1:26" ht="240.75" thickBot="1">
-      <c r="A54" s="27"/>
+    <row r="54" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A54" s="25"/>
       <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="6"/>
+      <c r="D54" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
@@ -3047,15 +3151,17 @@
       <c r="Y54" s="5"/>
       <c r="Z54" s="5"/>
     </row>
-    <row r="55" spans="1:26" ht="240.75" thickBot="1">
-      <c r="A55" s="27"/>
+    <row r="55" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A55" s="25"/>
       <c r="B55" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="6"/>
+      <c r="D55" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
@@ -3079,15 +3185,17 @@
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
     </row>
-    <row r="56" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A56" s="27"/>
+    <row r="56" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A56" s="25"/>
       <c r="B56" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="6"/>
+      <c r="D56" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
@@ -3111,15 +3219,17 @@
       <c r="Y56" s="5"/>
       <c r="Z56" s="5"/>
     </row>
-    <row r="57" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A57" s="27"/>
+    <row r="57" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A57" s="25"/>
       <c r="B57" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="6"/>
+      <c r="D57" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -3143,15 +3253,17 @@
       <c r="Y57" s="5"/>
       <c r="Z57" s="5"/>
     </row>
-    <row r="58" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A58" s="27"/>
+    <row r="58" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A58" s="25"/>
       <c r="B58" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="6"/>
+      <c r="D58" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
@@ -3175,15 +3287,17 @@
       <c r="Y58" s="5"/>
       <c r="Z58" s="5"/>
     </row>
-    <row r="59" spans="1:26" ht="210.75" thickBot="1">
-      <c r="A59" s="27"/>
+    <row r="59" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A59" s="25"/>
       <c r="B59" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="6"/>
+      <c r="D59" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
@@ -3207,15 +3321,17 @@
       <c r="Y59" s="5"/>
       <c r="Z59" s="5"/>
     </row>
-    <row r="60" spans="1:26" ht="240.75" thickBot="1">
-      <c r="A60" s="27"/>
+    <row r="60" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A60" s="25"/>
       <c r="B60" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="6"/>
+      <c r="D60" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -3239,15 +3355,17 @@
       <c r="Y60" s="5"/>
       <c r="Z60" s="5"/>
     </row>
-    <row r="61" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A61" s="27"/>
+    <row r="61" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A61" s="25"/>
       <c r="B61" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="6"/>
+      <c r="D61" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
@@ -3271,15 +3389,17 @@
       <c r="Y61" s="5"/>
       <c r="Z61" s="5"/>
     </row>
-    <row r="62" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A62" s="27"/>
+    <row r="62" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A62" s="25"/>
       <c r="B62" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="6"/>
+      <c r="D62" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -3303,15 +3423,17 @@
       <c r="Y62" s="5"/>
       <c r="Z62" s="5"/>
     </row>
-    <row r="63" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A63" s="27"/>
+    <row r="63" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A63" s="25"/>
       <c r="B63" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="6"/>
+      <c r="D63" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
@@ -3335,15 +3457,17 @@
       <c r="Y63" s="5"/>
       <c r="Z63" s="5"/>
     </row>
-    <row r="64" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A64" s="27"/>
+    <row r="64" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A64" s="25"/>
       <c r="B64" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="6"/>
+      <c r="D64" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -3367,15 +3491,17 @@
       <c r="Y64" s="5"/>
       <c r="Z64" s="5"/>
     </row>
-    <row r="65" spans="1:26" ht="225.75" thickBot="1">
-      <c r="A65" s="27"/>
+    <row r="65" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A65" s="25"/>
       <c r="B65" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="6"/>
+      <c r="D65" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
@@ -3399,15 +3525,17 @@
       <c r="Y65" s="5"/>
       <c r="Z65" s="5"/>
     </row>
-    <row r="66" spans="1:26" ht="270.75" thickBot="1">
-      <c r="A66" s="27"/>
+    <row r="66" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A66" s="25"/>
       <c r="B66" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="6"/>
+      <c r="D66" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -3431,15 +3559,17 @@
       <c r="Y66" s="5"/>
       <c r="Z66" s="5"/>
     </row>
-    <row r="67" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A67" s="27"/>
+    <row r="67" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A67" s="25"/>
       <c r="B67" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="6"/>
+      <c r="D67" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
@@ -3463,15 +3593,17 @@
       <c r="Y67" s="5"/>
       <c r="Z67" s="5"/>
     </row>
-    <row r="68" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A68" s="27"/>
+    <row r="68" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A68" s="25"/>
       <c r="B68" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="6"/>
+      <c r="D68" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
@@ -3495,15 +3627,17 @@
       <c r="Y68" s="5"/>
       <c r="Z68" s="5"/>
     </row>
-    <row r="69" spans="1:26" ht="30.75" thickBot="1">
-      <c r="A69" s="28"/>
+    <row r="69" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A69" s="21"/>
       <c r="B69" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D69" s="6"/>
+      <c r="D69" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
@@ -3527,8 +3661,8 @@
       <c r="Y69" s="5"/>
       <c r="Z69" s="5"/>
     </row>
-    <row r="70" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A70" s="26" t="s">
+    <row r="70" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A70" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B70" s="7" t="s">
@@ -3537,7 +3671,9 @@
       <c r="C70" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="6"/>
+      <c r="D70" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -3561,15 +3697,17 @@
       <c r="Y70" s="5"/>
       <c r="Z70" s="5"/>
     </row>
-    <row r="71" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A71" s="27"/>
+    <row r="71" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A71" s="25"/>
       <c r="B71" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D71" s="6"/>
+      <c r="D71" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
@@ -3593,15 +3731,17 @@
       <c r="Y71" s="5"/>
       <c r="Z71" s="5"/>
     </row>
-    <row r="72" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A72" s="27"/>
+    <row r="72" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A72" s="25"/>
       <c r="B72" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D72" s="6"/>
+      <c r="D72" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
@@ -3625,15 +3765,17 @@
       <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
     </row>
-    <row r="73" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A73" s="27"/>
+    <row r="73" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A73" s="25"/>
       <c r="B73" s="7" t="s">
         <v>81</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="6"/>
+      <c r="D73" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
@@ -3657,15 +3799,17 @@
       <c r="Y73" s="5"/>
       <c r="Z73" s="5"/>
     </row>
-    <row r="74" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A74" s="27"/>
+    <row r="74" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A74" s="25"/>
       <c r="B74" s="7" t="s">
         <v>82</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="6"/>
+      <c r="D74" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
@@ -3689,15 +3833,17 @@
       <c r="Y74" s="5"/>
       <c r="Z74" s="5"/>
     </row>
-    <row r="75" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A75" s="27"/>
+    <row r="75" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A75" s="25"/>
       <c r="B75" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="6"/>
+      <c r="D75" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
@@ -3721,15 +3867,17 @@
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
     </row>
-    <row r="76" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A76" s="28"/>
+    <row r="76" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A76" s="21"/>
       <c r="B76" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D76" s="6"/>
+      <c r="D76" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
@@ -3754,7 +3902,7 @@
       <c r="Z76" s="5"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A77" s="26" t="s">
+      <c r="A77" s="20" t="s">
         <v>85</v>
       </c>
       <c r="B77" s="6"/>
@@ -3783,15 +3931,17 @@
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
     </row>
-    <row r="78" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A78" s="27"/>
+    <row r="78" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A78" s="25"/>
       <c r="B78" s="6" t="s">
         <v>86</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D78" s="6"/>
+      <c r="D78" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
@@ -3815,15 +3965,17 @@
       <c r="Y78" s="5"/>
       <c r="Z78" s="5"/>
     </row>
-    <row r="79" spans="1:26" ht="129" thickBot="1">
-      <c r="A79" s="27"/>
+    <row r="79" spans="1:26" ht="27" thickBot="1">
+      <c r="A79" s="25"/>
       <c r="B79" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D79" s="6"/>
+      <c r="D79" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
@@ -3847,15 +3999,17 @@
       <c r="Y79" s="5"/>
       <c r="Z79" s="5"/>
     </row>
-    <row r="80" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A80" s="27"/>
+    <row r="80" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A80" s="25"/>
       <c r="B80" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="6"/>
+      <c r="D80" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
@@ -3879,15 +4033,17 @@
       <c r="Y80" s="5"/>
       <c r="Z80" s="5"/>
     </row>
-    <row r="81" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A81" s="27"/>
+    <row r="81" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A81" s="25"/>
       <c r="B81" s="6" t="s">
         <v>89</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="6"/>
+      <c r="D81" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
@@ -3911,15 +4067,17 @@
       <c r="Y81" s="5"/>
       <c r="Z81" s="5"/>
     </row>
-    <row r="82" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A82" s="27"/>
+    <row r="82" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A82" s="25"/>
       <c r="B82" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D82" s="6"/>
+      <c r="D82" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
@@ -3943,15 +4101,17 @@
       <c r="Y82" s="5"/>
       <c r="Z82" s="5"/>
     </row>
-    <row r="83" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A83" s="27"/>
+    <row r="83" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A83" s="25"/>
       <c r="B83" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D83" s="6"/>
+      <c r="D83" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
@@ -3975,15 +4135,17 @@
       <c r="Y83" s="5"/>
       <c r="Z83" s="5"/>
     </row>
-    <row r="84" spans="1:26" ht="129" thickBot="1">
-      <c r="A84" s="27"/>
+    <row r="84" spans="1:26" ht="27" thickBot="1">
+      <c r="A84" s="25"/>
       <c r="B84" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D84" s="6"/>
+      <c r="D84" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
@@ -4007,15 +4169,17 @@
       <c r="Y84" s="5"/>
       <c r="Z84" s="5"/>
     </row>
-    <row r="85" spans="1:26" ht="129" thickBot="1">
-      <c r="A85" s="27"/>
+    <row r="85" spans="1:26" ht="27" thickBot="1">
+      <c r="A85" s="25"/>
       <c r="B85" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D85" s="6"/>
+      <c r="D85" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
@@ -4039,15 +4203,17 @@
       <c r="Y85" s="5"/>
       <c r="Z85" s="5"/>
     </row>
-    <row r="86" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A86" s="27"/>
+    <row r="86" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A86" s="25"/>
       <c r="B86" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D86" s="6"/>
+      <c r="D86" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
@@ -4071,15 +4237,17 @@
       <c r="Y86" s="5"/>
       <c r="Z86" s="5"/>
     </row>
-    <row r="87" spans="1:26" ht="141.75" thickBot="1">
-      <c r="A87" s="27"/>
+    <row r="87" spans="1:26" ht="27" thickBot="1">
+      <c r="A87" s="25"/>
       <c r="B87" s="6" t="s">
         <v>95</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D87" s="6"/>
+      <c r="D87" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
@@ -4103,15 +4271,17 @@
       <c r="Y87" s="5"/>
       <c r="Z87" s="5"/>
     </row>
-    <row r="88" spans="1:26" ht="129" thickBot="1">
-      <c r="A88" s="27"/>
+    <row r="88" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A88" s="25"/>
       <c r="B88" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D88" s="6"/>
+      <c r="D88" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
@@ -4135,15 +4305,17 @@
       <c r="Y88" s="5"/>
       <c r="Z88" s="5"/>
     </row>
-    <row r="89" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A89" s="27"/>
+    <row r="89" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A89" s="25"/>
       <c r="B89" s="7" t="s">
         <v>97</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D89" s="6"/>
+      <c r="D89" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
@@ -4167,15 +4339,17 @@
       <c r="Y89" s="5"/>
       <c r="Z89" s="5"/>
     </row>
-    <row r="90" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A90" s="27"/>
+    <row r="90" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A90" s="25"/>
       <c r="B90" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="6"/>
+      <c r="D90" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -4199,15 +4373,17 @@
       <c r="Y90" s="5"/>
       <c r="Z90" s="5"/>
     </row>
-    <row r="91" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A91" s="27"/>
+    <row r="91" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A91" s="25"/>
       <c r="B91" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D91" s="6"/>
+      <c r="D91" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -4231,15 +4407,17 @@
       <c r="Y91" s="5"/>
       <c r="Z91" s="5"/>
     </row>
-    <row r="92" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A92" s="27"/>
+    <row r="92" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A92" s="25"/>
       <c r="B92" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="6"/>
+      <c r="D92" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -4263,15 +4441,17 @@
       <c r="Y92" s="5"/>
       <c r="Z92" s="5"/>
     </row>
-    <row r="93" spans="1:26" ht="103.5" thickBot="1">
-      <c r="A93" s="27"/>
+    <row r="93" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A93" s="25"/>
       <c r="B93" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D93" s="6"/>
+      <c r="D93" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
@@ -4295,15 +4475,17 @@
       <c r="Y93" s="5"/>
       <c r="Z93" s="5"/>
     </row>
-    <row r="94" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A94" s="27"/>
+    <row r="94" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A94" s="25"/>
       <c r="B94" s="6" t="s">
         <v>102</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="6"/>
+      <c r="D94" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
@@ -4327,15 +4509,17 @@
       <c r="Y94" s="5"/>
       <c r="Z94" s="5"/>
     </row>
-    <row r="95" spans="1:26" ht="65.25" thickBot="1">
-      <c r="A95" s="27"/>
+    <row r="95" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A95" s="25"/>
       <c r="B95" s="6" t="s">
         <v>103</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D95" s="6"/>
+      <c r="D95" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
@@ -4359,15 +4543,17 @@
       <c r="Y95" s="5"/>
       <c r="Z95" s="5"/>
     </row>
-    <row r="96" spans="1:26" ht="78" thickBot="1">
-      <c r="A96" s="27"/>
+    <row r="96" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A96" s="25"/>
       <c r="B96" s="6" t="s">
         <v>104</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D96" s="6"/>
+      <c r="D96" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
@@ -4391,15 +4577,17 @@
       <c r="Y96" s="5"/>
       <c r="Z96" s="5"/>
     </row>
-    <row r="97" spans="1:26" ht="65.25" thickBot="1">
-      <c r="A97" s="27"/>
+    <row r="97" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A97" s="25"/>
       <c r="B97" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D97" s="6"/>
+      <c r="D97" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
@@ -4423,15 +4611,17 @@
       <c r="Y97" s="5"/>
       <c r="Z97" s="5"/>
     </row>
-    <row r="98" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A98" s="27"/>
+    <row r="98" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A98" s="25"/>
       <c r="B98" s="6" t="s">
         <v>106</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D98" s="6"/>
+      <c r="D98" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
@@ -4456,7 +4646,7 @@
       <c r="Z98" s="5"/>
     </row>
     <row r="99" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A99" s="27"/>
+      <c r="A99" s="25"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
@@ -4483,15 +4673,17 @@
       <c r="Y99" s="5"/>
       <c r="Z99" s="5"/>
     </row>
-    <row r="100" spans="1:26" ht="141.75" thickBot="1">
-      <c r="A100" s="27"/>
+    <row r="100" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A100" s="25"/>
       <c r="B100" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D100" s="6"/>
+      <c r="D100" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
@@ -4515,15 +4707,17 @@
       <c r="Y100" s="5"/>
       <c r="Z100" s="5"/>
     </row>
-    <row r="101" spans="1:26" ht="141.75" thickBot="1">
-      <c r="A101" s="27"/>
+    <row r="101" spans="1:26" ht="27" thickBot="1">
+      <c r="A101" s="25"/>
       <c r="B101" s="6" t="s">
         <v>108</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D101" s="6"/>
+      <c r="D101" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
@@ -4547,15 +4741,17 @@
       <c r="Y101" s="5"/>
       <c r="Z101" s="5"/>
     </row>
-    <row r="102" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A102" s="27"/>
+    <row r="102" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A102" s="25"/>
       <c r="B102" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D102" s="6"/>
+      <c r="D102" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
@@ -4580,10 +4776,12 @@
       <c r="Z102" s="5"/>
     </row>
     <row r="103" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A103" s="27"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
+      <c r="D103" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
@@ -4607,15 +4805,17 @@
       <c r="Y103" s="5"/>
       <c r="Z103" s="5"/>
     </row>
-    <row r="104" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A104" s="27"/>
+    <row r="104" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A104" s="25"/>
       <c r="B104" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="6"/>
+      <c r="D104" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
@@ -4639,15 +4839,17 @@
       <c r="Y104" s="5"/>
       <c r="Z104" s="5"/>
     </row>
-    <row r="105" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A105" s="27"/>
+    <row r="105" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A105" s="25"/>
       <c r="B105" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="6"/>
+      <c r="D105" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
@@ -4671,15 +4873,17 @@
       <c r="Y105" s="5"/>
       <c r="Z105" s="5"/>
     </row>
-    <row r="106" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A106" s="27"/>
+    <row r="106" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A106" s="25"/>
       <c r="B106" s="7" t="s">
         <v>112</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D106" s="6"/>
+      <c r="D106" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
@@ -4703,15 +4907,17 @@
       <c r="Y106" s="5"/>
       <c r="Z106" s="5"/>
     </row>
-    <row r="107" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A107" s="27"/>
+    <row r="107" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A107" s="25"/>
       <c r="B107" s="7" t="s">
         <v>113</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D107" s="6"/>
+      <c r="D107" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
@@ -4735,15 +4941,17 @@
       <c r="Y107" s="5"/>
       <c r="Z107" s="5"/>
     </row>
-    <row r="108" spans="1:26" ht="167.25" thickBot="1">
-      <c r="A108" s="27"/>
+    <row r="108" spans="1:26" ht="27" thickBot="1">
+      <c r="A108" s="25"/>
       <c r="B108" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D108" s="6"/>
+      <c r="D108" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
@@ -4767,15 +4975,17 @@
       <c r="Y108" s="5"/>
       <c r="Z108" s="5"/>
     </row>
-    <row r="109" spans="1:26" ht="103.5" thickBot="1">
-      <c r="A109" s="27"/>
+    <row r="109" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A109" s="25"/>
       <c r="B109" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D109" s="6"/>
+      <c r="D109" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
@@ -4799,15 +5009,17 @@
       <c r="Y109" s="5"/>
       <c r="Z109" s="5"/>
     </row>
-    <row r="110" spans="1:26" ht="141.75" thickBot="1">
-      <c r="A110" s="27"/>
+    <row r="110" spans="1:26" ht="27" thickBot="1">
+      <c r="A110" s="25"/>
       <c r="B110" s="6" t="s">
         <v>116</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D110" s="6"/>
+      <c r="D110" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
@@ -4831,15 +5043,17 @@
       <c r="Y110" s="5"/>
       <c r="Z110" s="5"/>
     </row>
-    <row r="111" spans="1:26" ht="65.25" thickBot="1">
-      <c r="A111" s="27"/>
+    <row r="111" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A111" s="25"/>
       <c r="B111" s="6" t="s">
         <v>117</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D111" s="6"/>
+      <c r="D111" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
@@ -4863,15 +5077,17 @@
       <c r="Y111" s="5"/>
       <c r="Z111" s="5"/>
     </row>
-    <row r="112" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A112" s="27"/>
+    <row r="112" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A112" s="25"/>
       <c r="B112" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D112" s="6"/>
+      <c r="D112" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
@@ -4895,15 +5111,17 @@
       <c r="Y112" s="5"/>
       <c r="Z112" s="5"/>
     </row>
-    <row r="113" spans="1:26" ht="52.5" thickBot="1">
-      <c r="A113" s="27"/>
+    <row r="113" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A113" s="25"/>
       <c r="B113" s="6" t="s">
         <v>119</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D113" s="6"/>
+      <c r="D113" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
@@ -4927,15 +5145,17 @@
       <c r="Y113" s="5"/>
       <c r="Z113" s="5"/>
     </row>
-    <row r="114" spans="1:26" ht="116.25" thickBot="1">
-      <c r="A114" s="27"/>
+    <row r="114" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A114" s="25"/>
       <c r="B114" s="6" t="s">
         <v>120</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D114" s="6"/>
+      <c r="D114" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
@@ -4959,15 +5179,17 @@
       <c r="Y114" s="5"/>
       <c r="Z114" s="5"/>
     </row>
-    <row r="115" spans="1:26" ht="154.5" thickBot="1">
-      <c r="A115" s="27"/>
+    <row r="115" spans="1:26" ht="27" thickBot="1">
+      <c r="A115" s="25"/>
       <c r="B115" s="6" t="s">
         <v>121</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D115" s="6"/>
+      <c r="D115" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
       <c r="G115" s="5"/>
@@ -4991,15 +5213,17 @@
       <c r="Y115" s="5"/>
       <c r="Z115" s="5"/>
     </row>
-    <row r="116" spans="1:26" ht="150.75" thickBot="1">
-      <c r="A116" s="27"/>
+    <row r="116" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A116" s="25"/>
       <c r="B116" s="7" t="s">
         <v>122</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D116" s="6"/>
+      <c r="D116" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E116" s="5"/>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
@@ -5023,15 +5247,17 @@
       <c r="Y116" s="5"/>
       <c r="Z116" s="5"/>
     </row>
-    <row r="117" spans="1:26" ht="65.25" thickBot="1">
-      <c r="A117" s="27"/>
+    <row r="117" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A117" s="25"/>
       <c r="B117" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D117" s="6"/>
+      <c r="D117" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
@@ -5055,15 +5281,17 @@
       <c r="Y117" s="5"/>
       <c r="Z117" s="5"/>
     </row>
-    <row r="118" spans="1:26" ht="65.25" thickBot="1">
-      <c r="A118" s="27"/>
+    <row r="118" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A118" s="25"/>
       <c r="B118" s="6" t="s">
         <v>124</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D118" s="6"/>
+      <c r="D118" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
@@ -5088,7 +5316,7 @@
       <c r="Z118" s="5"/>
     </row>
     <row r="119" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A119" s="27"/>
+      <c r="A119" s="25"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
@@ -5115,15 +5343,17 @@
       <c r="Y119" s="5"/>
       <c r="Z119" s="5"/>
     </row>
-    <row r="120" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A120" s="27"/>
+    <row r="120" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A120" s="25"/>
       <c r="B120" s="7" t="s">
         <v>125</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D120" s="6"/>
+      <c r="D120" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
@@ -5147,15 +5377,17 @@
       <c r="Y120" s="5"/>
       <c r="Z120" s="5"/>
     </row>
-    <row r="121" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A121" s="27"/>
+    <row r="121" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A121" s="25"/>
       <c r="B121" s="7" t="s">
         <v>126</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D121" s="6"/>
+      <c r="D121" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
@@ -5179,15 +5411,17 @@
       <c r="Y121" s="5"/>
       <c r="Z121" s="5"/>
     </row>
-    <row r="122" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A122" s="27"/>
+    <row r="122" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A122" s="25"/>
       <c r="B122" s="7" t="s">
         <v>127</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D122" s="6"/>
+      <c r="D122" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
@@ -5211,15 +5445,17 @@
       <c r="Y122" s="5"/>
       <c r="Z122" s="5"/>
     </row>
-    <row r="123" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A123" s="27"/>
+    <row r="123" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A123" s="25"/>
       <c r="B123" s="7" t="s">
         <v>128</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D123" s="6"/>
+      <c r="D123" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
@@ -5243,15 +5479,17 @@
       <c r="Y123" s="5"/>
       <c r="Z123" s="5"/>
     </row>
-    <row r="124" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A124" s="27"/>
+    <row r="124" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A124" s="25"/>
       <c r="B124" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D124" s="6"/>
+      <c r="D124" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
       <c r="G124" s="5"/>
@@ -5275,15 +5513,17 @@
       <c r="Y124" s="5"/>
       <c r="Z124" s="5"/>
     </row>
-    <row r="125" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A125" s="27"/>
+    <row r="125" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A125" s="25"/>
       <c r="B125" s="7" t="s">
         <v>130</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D125" s="6"/>
+      <c r="D125" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
@@ -5307,15 +5547,17 @@
       <c r="Y125" s="5"/>
       <c r="Z125" s="5"/>
     </row>
-    <row r="126" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A126" s="27"/>
+    <row r="126" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A126" s="25"/>
       <c r="B126" s="7" t="s">
         <v>131</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D126" s="6"/>
+      <c r="D126" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E126" s="5"/>
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
@@ -5339,15 +5581,17 @@
       <c r="Y126" s="5"/>
       <c r="Z126" s="5"/>
     </row>
-    <row r="127" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A127" s="27"/>
+    <row r="127" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A127" s="25"/>
       <c r="B127" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D127" s="6"/>
+      <c r="D127" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
       <c r="G127" s="5"/>
@@ -5371,15 +5615,17 @@
       <c r="Y127" s="5"/>
       <c r="Z127" s="5"/>
     </row>
-    <row r="128" spans="1:26" ht="129" thickBot="1">
-      <c r="A128" s="27"/>
+    <row r="128" spans="1:26" ht="27" thickBot="1">
+      <c r="A128" s="25"/>
       <c r="B128" s="6" t="s">
         <v>133</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D128" s="6"/>
+      <c r="D128" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
@@ -5403,15 +5649,17 @@
       <c r="Y128" s="5"/>
       <c r="Z128" s="5"/>
     </row>
-    <row r="129" spans="1:26" ht="231" thickBot="1">
-      <c r="A129" s="27"/>
+    <row r="129" spans="1:26" ht="27" thickBot="1">
+      <c r="A129" s="25"/>
       <c r="B129" s="6" t="s">
         <v>134</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D129" s="6"/>
+      <c r="D129" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
@@ -5435,15 +5683,17 @@
       <c r="Y129" s="5"/>
       <c r="Z129" s="5"/>
     </row>
-    <row r="130" spans="1:26" ht="154.5" thickBot="1">
-      <c r="A130" s="27"/>
+    <row r="130" spans="1:26" ht="27" thickBot="1">
+      <c r="A130" s="25"/>
       <c r="B130" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D130" s="6"/>
+      <c r="D130" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
@@ -5468,7 +5718,7 @@
       <c r="Z130" s="5"/>
     </row>
     <row r="131" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A131" s="28"/>
+      <c r="A131" s="21"/>
       <c r="B131" s="6"/>
       <c r="C131" s="6"/>
       <c r="D131" s="6"/>
@@ -5496,9 +5746,9 @@
       <c r="Z131" s="5"/>
     </row>
     <row r="132" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A132" s="20"/>
-      <c r="B132" s="21"/>
-      <c r="C132" s="22"/>
+      <c r="A132" s="17"/>
+      <c r="B132" s="18"/>
+      <c r="C132" s="19"/>
       <c r="D132" s="6"/>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
@@ -5523,8 +5773,8 @@
       <c r="Y132" s="5"/>
       <c r="Z132" s="5"/>
     </row>
-    <row r="133" spans="1:26" ht="135.75" thickBot="1">
-      <c r="A133" s="26" t="s">
+    <row r="133" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A133" s="20" t="s">
         <v>136</v>
       </c>
       <c r="B133" s="7" t="s">
@@ -5533,7 +5783,9 @@
       <c r="C133" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D133" s="6"/>
+      <c r="D133" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
       <c r="G133" s="5"/>
@@ -5557,15 +5809,17 @@
       <c r="Y133" s="5"/>
       <c r="Z133" s="5"/>
     </row>
-    <row r="134" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A134" s="27"/>
+    <row r="134" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A134" s="25"/>
       <c r="B134" s="7" t="s">
         <v>138</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="6"/>
+      <c r="D134" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
       <c r="G134" s="5"/>
@@ -5589,15 +5843,17 @@
       <c r="Y134" s="5"/>
       <c r="Z134" s="5"/>
     </row>
-    <row r="135" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A135" s="27"/>
+    <row r="135" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A135" s="25"/>
       <c r="B135" s="7" t="s">
         <v>139</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D135" s="6"/>
+      <c r="D135" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
       <c r="G135" s="5"/>
@@ -5621,15 +5877,17 @@
       <c r="Y135" s="5"/>
       <c r="Z135" s="5"/>
     </row>
-    <row r="136" spans="1:26" ht="150.75" thickBot="1">
-      <c r="A136" s="27"/>
+    <row r="136" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A136" s="25"/>
       <c r="B136" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C136" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D136" s="6"/>
+      <c r="D136" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
@@ -5653,15 +5911,17 @@
       <c r="Y136" s="5"/>
       <c r="Z136" s="5"/>
     </row>
-    <row r="137" spans="1:26" ht="180.75" thickBot="1">
-      <c r="A137" s="28"/>
+    <row r="137" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A137" s="21"/>
       <c r="B137" s="7" t="s">
         <v>141</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D137" s="6"/>
+      <c r="D137" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
@@ -5686,9 +5946,9 @@
       <c r="Z137" s="5"/>
     </row>
     <row r="138" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A138" s="20"/>
-      <c r="B138" s="21"/>
-      <c r="C138" s="22"/>
+      <c r="A138" s="17"/>
+      <c r="B138" s="18"/>
+      <c r="C138" s="19"/>
       <c r="D138" s="6"/>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
@@ -5713,8 +5973,8 @@
       <c r="Y138" s="5"/>
       <c r="Z138" s="5"/>
     </row>
-    <row r="139" spans="1:26" ht="45.75" thickBot="1">
-      <c r="A139" s="26" t="s">
+    <row r="139" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A139" s="20" t="s">
         <v>142</v>
       </c>
       <c r="B139" s="12" t="s">
@@ -5723,7 +5983,9 @@
       <c r="C139" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D139" s="6"/>
+      <c r="D139" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
       <c r="G139" s="5"/>
@@ -5747,15 +6009,17 @@
       <c r="Y139" s="5"/>
       <c r="Z139" s="5"/>
     </row>
-    <row r="140" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A140" s="27"/>
+    <row r="140" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A140" s="25"/>
       <c r="B140" s="7" t="s">
         <v>144</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D140" s="6"/>
+      <c r="D140" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
@@ -5779,15 +6043,17 @@
       <c r="Y140" s="5"/>
       <c r="Z140" s="5"/>
     </row>
-    <row r="141" spans="1:26" ht="165.75" thickBot="1">
-      <c r="A141" s="29"/>
+    <row r="141" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A141" s="26"/>
       <c r="B141" s="13" t="s">
         <v>61</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D141" s="6"/>
+      <c r="D141" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
       <c r="G141" s="5"/>
@@ -5812,9 +6078,9 @@
       <c r="Z141" s="5"/>
     </row>
     <row r="142" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A142" s="30"/>
-      <c r="B142" s="31"/>
-      <c r="C142" s="32"/>
+      <c r="A142" s="27"/>
+      <c r="B142" s="28"/>
+      <c r="C142" s="29"/>
       <c r="D142" s="6"/>
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
@@ -5839,8 +6105,8 @@
       <c r="Y142" s="5"/>
       <c r="Z142" s="5"/>
     </row>
-    <row r="143" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A143" s="26" t="s">
+    <row r="143" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A143" s="20" t="s">
         <v>145</v>
       </c>
       <c r="B143" s="7" t="s">
@@ -5849,7 +6115,9 @@
       <c r="C143" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D143" s="6"/>
+      <c r="D143" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
       <c r="G143" s="5"/>
@@ -5873,15 +6141,17 @@
       <c r="Y143" s="5"/>
       <c r="Z143" s="5"/>
     </row>
-    <row r="144" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A144" s="28"/>
+    <row r="144" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A144" s="21"/>
       <c r="B144" s="7" t="s">
         <v>147</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D144" s="6"/>
+      <c r="D144" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E144" s="5"/>
       <c r="F144" s="5"/>
       <c r="G144" s="5"/>
@@ -5906,9 +6176,9 @@
       <c r="Z144" s="5"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A145" s="20"/>
-      <c r="B145" s="21"/>
-      <c r="C145" s="22"/>
+      <c r="A145" s="17"/>
+      <c r="B145" s="18"/>
+      <c r="C145" s="19"/>
       <c r="D145" s="6"/>
       <c r="E145" s="5"/>
       <c r="F145" s="5"/>
@@ -5933,8 +6203,8 @@
       <c r="Y145" s="5"/>
       <c r="Z145" s="5"/>
     </row>
-    <row r="146" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A146" s="26" t="s">
+    <row r="146" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A146" s="20" t="s">
         <v>148</v>
       </c>
       <c r="B146" s="7" t="s">
@@ -5943,7 +6213,9 @@
       <c r="C146" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D146" s="6"/>
+      <c r="D146" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
       <c r="G146" s="5"/>
@@ -5967,15 +6239,17 @@
       <c r="Y146" s="5"/>
       <c r="Z146" s="5"/>
     </row>
-    <row r="147" spans="1:26" ht="115.5" thickBot="1">
-      <c r="A147" s="28"/>
+    <row r="147" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A147" s="21"/>
       <c r="B147" s="14" t="s">
         <v>150</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D147" s="6"/>
+      <c r="D147" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E147" s="5"/>
       <c r="F147" s="5"/>
       <c r="G147" s="5"/>
@@ -5999,7 +6273,7 @@
       <c r="Y147" s="5"/>
       <c r="Z147" s="5"/>
     </row>
-    <row r="148" spans="1:26" ht="60.75" thickBot="1">
+    <row r="148" spans="1:26" ht="15.75" thickBot="1">
       <c r="A148" s="15"/>
       <c r="B148" s="7" t="s">
         <v>151</v>
@@ -6007,7 +6281,9 @@
       <c r="C148" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D148" s="6"/>
+      <c r="D148" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
       <c r="G148" s="5"/>
@@ -6031,8 +6307,8 @@
       <c r="Y148" s="5"/>
       <c r="Z148" s="5"/>
     </row>
-    <row r="149" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A149" s="33" t="s">
+    <row r="149" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A149" s="22" t="s">
         <v>152</v>
       </c>
       <c r="B149" s="16" t="s">
@@ -6041,7 +6317,9 @@
       <c r="C149" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D149" s="6"/>
+      <c r="D149" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
       <c r="G149" s="5"/>
@@ -6065,15 +6343,17 @@
       <c r="Y149" s="5"/>
       <c r="Z149" s="5"/>
     </row>
-    <row r="150" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A150" s="34"/>
+    <row r="150" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A150" s="23"/>
       <c r="B150" s="16" t="s">
         <v>154</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D150" s="6"/>
+      <c r="D150" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E150" s="5"/>
       <c r="F150" s="5"/>
       <c r="G150" s="5"/>
@@ -6097,15 +6377,17 @@
       <c r="Y150" s="5"/>
       <c r="Z150" s="5"/>
     </row>
-    <row r="151" spans="1:26" ht="150.75" thickBot="1">
-      <c r="A151" s="34"/>
+    <row r="151" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A151" s="23"/>
       <c r="B151" s="16" t="s">
         <v>155</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D151" s="6"/>
+      <c r="D151" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E151" s="5"/>
       <c r="F151" s="5"/>
       <c r="G151" s="5"/>
@@ -6129,15 +6411,17 @@
       <c r="Y151" s="5"/>
       <c r="Z151" s="5"/>
     </row>
-    <row r="152" spans="1:26" ht="150.75" thickBot="1">
-      <c r="A152" s="34"/>
+    <row r="152" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A152" s="23"/>
       <c r="B152" s="16" t="s">
         <v>156</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D152" s="6"/>
+      <c r="D152" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E152" s="5"/>
       <c r="F152" s="5"/>
       <c r="G152" s="5"/>
@@ -6161,15 +6445,17 @@
       <c r="Y152" s="5"/>
       <c r="Z152" s="5"/>
     </row>
-    <row r="153" spans="1:26" ht="150.75" thickBot="1">
-      <c r="A153" s="34"/>
+    <row r="153" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A153" s="23"/>
       <c r="B153" s="16" t="s">
         <v>157</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D153" s="6"/>
+      <c r="D153" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
       <c r="G153" s="5"/>
@@ -6193,15 +6479,17 @@
       <c r="Y153" s="5"/>
       <c r="Z153" s="5"/>
     </row>
-    <row r="154" spans="1:26" ht="180.75" thickBot="1">
-      <c r="A154" s="34"/>
+    <row r="154" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A154" s="23"/>
       <c r="B154" s="16" t="s">
         <v>158</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D154" s="6"/>
+      <c r="D154" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E154" s="5"/>
       <c r="F154" s="5"/>
       <c r="G154" s="5"/>
@@ -6225,15 +6513,17 @@
       <c r="Y154" s="5"/>
       <c r="Z154" s="5"/>
     </row>
-    <row r="155" spans="1:26" ht="165.75" thickBot="1">
-      <c r="A155" s="34"/>
+    <row r="155" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A155" s="23"/>
       <c r="B155" s="16" t="s">
         <v>159</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D155" s="6"/>
+      <c r="D155" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
       <c r="G155" s="5"/>
@@ -6257,15 +6547,17 @@
       <c r="Y155" s="5"/>
       <c r="Z155" s="5"/>
     </row>
-    <row r="156" spans="1:26" ht="285.75" thickBot="1">
-      <c r="A156" s="34"/>
+    <row r="156" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A156" s="23"/>
       <c r="B156" s="16" t="s">
         <v>160</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D156" s="6"/>
+      <c r="D156" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
       <c r="G156" s="5"/>
@@ -6289,15 +6581,17 @@
       <c r="Y156" s="5"/>
       <c r="Z156" s="5"/>
     </row>
-    <row r="157" spans="1:26" ht="270.75" thickBot="1">
-      <c r="A157" s="35"/>
+    <row r="157" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A157" s="24"/>
       <c r="B157" s="16" t="s">
         <v>161</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D157" s="6"/>
+      <c r="D157" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E157" s="5"/>
       <c r="F157" s="5"/>
       <c r="G157" s="5"/>
@@ -6321,8 +6615,8 @@
       <c r="Y157" s="5"/>
       <c r="Z157" s="5"/>
     </row>
-    <row r="158" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A158" s="33" t="s">
+    <row r="158" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A158" s="22" t="s">
         <v>162</v>
       </c>
       <c r="B158" s="16" t="s">
@@ -6331,7 +6625,9 @@
       <c r="C158" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D158" s="6"/>
+      <c r="D158" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E158" s="5"/>
       <c r="F158" s="5"/>
       <c r="G158" s="5"/>
@@ -6356,14 +6652,16 @@
       <c r="Z158" s="5"/>
     </row>
     <row r="159" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A159" s="34"/>
+      <c r="A159" s="23"/>
       <c r="B159" s="16" t="s">
         <v>164</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D159" s="6"/>
+      <c r="D159" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E159" s="5"/>
       <c r="F159" s="5"/>
       <c r="G159" s="5"/>
@@ -6387,15 +6685,17 @@
       <c r="Y159" s="5"/>
       <c r="Z159" s="5"/>
     </row>
-    <row r="160" spans="1:26" ht="30.75" thickBot="1">
-      <c r="A160" s="34"/>
+    <row r="160" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A160" s="23"/>
       <c r="B160" s="7" t="s">
         <v>165</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D160" s="6"/>
+      <c r="D160" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E160" s="5"/>
       <c r="F160" s="5"/>
       <c r="G160" s="5"/>
@@ -6419,15 +6719,17 @@
       <c r="Y160" s="5"/>
       <c r="Z160" s="5"/>
     </row>
-    <row r="161" spans="1:26" ht="135.75" thickBot="1">
-      <c r="A161" s="34"/>
+    <row r="161" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A161" s="23"/>
       <c r="B161" s="16" t="s">
         <v>166</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D161" s="6"/>
+      <c r="D161" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E161" s="5"/>
       <c r="F161" s="5"/>
       <c r="G161" s="5"/>
@@ -6451,15 +6753,17 @@
       <c r="Y161" s="5"/>
       <c r="Z161" s="5"/>
     </row>
-    <row r="162" spans="1:26" ht="375.75" thickBot="1">
-      <c r="A162" s="34"/>
+    <row r="162" spans="1:26" ht="45.75" thickBot="1">
+      <c r="A162" s="23"/>
       <c r="B162" s="16" t="s">
         <v>167</v>
       </c>
       <c r="C162" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D162" s="6"/>
+      <c r="D162" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E162" s="5"/>
       <c r="F162" s="5"/>
       <c r="G162" s="5"/>
@@ -6483,15 +6787,17 @@
       <c r="Y162" s="5"/>
       <c r="Z162" s="5"/>
     </row>
-    <row r="163" spans="1:26" ht="150.75" thickBot="1">
-      <c r="A163" s="34"/>
+    <row r="163" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A163" s="23"/>
       <c r="B163" s="16" t="s">
         <v>168</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D163" s="6"/>
+      <c r="D163" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E163" s="5"/>
       <c r="F163" s="5"/>
       <c r="G163" s="5"/>
@@ -6515,15 +6821,17 @@
       <c r="Y163" s="5"/>
       <c r="Z163" s="5"/>
     </row>
-    <row r="164" spans="1:26" ht="120.75" thickBot="1">
-      <c r="A164" s="34"/>
+    <row r="164" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A164" s="23"/>
       <c r="B164" s="16" t="s">
         <v>169</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D164" s="6"/>
+      <c r="D164" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E164" s="5"/>
       <c r="F164" s="5"/>
       <c r="G164" s="5"/>
@@ -6547,15 +6855,17 @@
       <c r="Y164" s="5"/>
       <c r="Z164" s="5"/>
     </row>
-    <row r="165" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A165" s="35"/>
+    <row r="165" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A165" s="24"/>
       <c r="B165" s="16" t="s">
         <v>170</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D165" s="6"/>
+      <c r="D165" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E165" s="5"/>
       <c r="F165" s="5"/>
       <c r="G165" s="5"/>
@@ -6579,8 +6889,8 @@
       <c r="Y165" s="5"/>
       <c r="Z165" s="5"/>
     </row>
-    <row r="166" spans="1:26" ht="195.75" thickBot="1">
-      <c r="A166" s="33" t="s">
+    <row r="166" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A166" s="22" t="s">
         <v>171</v>
       </c>
       <c r="B166" s="7" t="s">
@@ -6589,7 +6899,9 @@
       <c r="C166" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D166" s="6"/>
+      <c r="D166" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E166" s="5"/>
       <c r="F166" s="5"/>
       <c r="G166" s="5"/>
@@ -6613,15 +6925,17 @@
       <c r="Y166" s="5"/>
       <c r="Z166" s="5"/>
     </row>
-    <row r="167" spans="1:26" ht="60.75" thickBot="1">
-      <c r="A167" s="34"/>
+    <row r="167" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A167" s="23"/>
       <c r="B167" s="16" t="s">
         <v>173</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D167" s="6"/>
+      <c r="D167" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E167" s="5"/>
       <c r="F167" s="5"/>
       <c r="G167" s="5"/>
@@ -6645,15 +6959,17 @@
       <c r="Y167" s="5"/>
       <c r="Z167" s="5"/>
     </row>
-    <row r="168" spans="1:26" ht="90.75" thickBot="1">
-      <c r="A168" s="34"/>
+    <row r="168" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A168" s="23"/>
       <c r="B168" s="7" t="s">
         <v>174</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D168" s="6"/>
+      <c r="D168" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E168" s="5"/>
       <c r="F168" s="5"/>
       <c r="G168" s="5"/>
@@ -6677,15 +6993,17 @@
       <c r="Y168" s="5"/>
       <c r="Z168" s="5"/>
     </row>
-    <row r="169" spans="1:26" ht="180.75" thickBot="1">
-      <c r="A169" s="34"/>
+    <row r="169" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A169" s="23"/>
       <c r="B169" s="7" t="s">
         <v>175</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D169" s="6"/>
+      <c r="D169" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E169" s="5"/>
       <c r="F169" s="5"/>
       <c r="G169" s="5"/>
@@ -6709,15 +7027,17 @@
       <c r="Y169" s="5"/>
       <c r="Z169" s="5"/>
     </row>
-    <row r="170" spans="1:26" ht="75.75" thickBot="1">
-      <c r="A170" s="34"/>
+    <row r="170" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A170" s="23"/>
       <c r="B170" s="7" t="s">
         <v>176</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D170" s="6"/>
+      <c r="D170" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E170" s="5"/>
       <c r="F170" s="5"/>
       <c r="G170" s="5"/>
@@ -6741,15 +7061,17 @@
       <c r="Y170" s="5"/>
       <c r="Z170" s="5"/>
     </row>
-    <row r="171" spans="1:26" ht="285.75" thickBot="1">
-      <c r="A171" s="34"/>
+    <row r="171" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A171" s="23"/>
       <c r="B171" s="7" t="s">
         <v>177</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D171" s="6"/>
+      <c r="D171" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E171" s="5"/>
       <c r="F171" s="5"/>
       <c r="G171" s="5"/>
@@ -6773,15 +7095,17 @@
       <c r="Y171" s="5"/>
       <c r="Z171" s="5"/>
     </row>
-    <row r="172" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A172" s="34"/>
+    <row r="172" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A172" s="23"/>
       <c r="B172" s="7" t="s">
         <v>178</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D172" s="6"/>
+      <c r="D172" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="E172" s="5"/>
       <c r="F172" s="5"/>
       <c r="G172" s="5"/>
@@ -6805,15 +7129,17 @@
       <c r="Y172" s="5"/>
       <c r="Z172" s="5"/>
     </row>
-    <row r="173" spans="1:26" ht="103.5" thickBot="1">
-      <c r="A173" s="34"/>
+    <row r="173" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A173" s="23"/>
       <c r="B173" s="6" t="s">
         <v>179</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D173" s="6"/>
+      <c r="D173" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E173" s="5"/>
       <c r="F173" s="5"/>
       <c r="G173" s="5"/>
@@ -6837,15 +7163,17 @@
       <c r="Y173" s="5"/>
       <c r="Z173" s="5"/>
     </row>
-    <row r="174" spans="1:26" ht="105.75" thickBot="1">
-      <c r="A174" s="34"/>
+    <row r="174" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A174" s="23"/>
       <c r="B174" s="7" t="s">
         <v>180</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D174" s="6"/>
+      <c r="D174" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E174" s="5"/>
       <c r="F174" s="5"/>
       <c r="G174" s="5"/>
@@ -6869,15 +7197,17 @@
       <c r="Y174" s="5"/>
       <c r="Z174" s="5"/>
     </row>
-    <row r="175" spans="1:26" ht="195.75" thickBot="1">
-      <c r="A175" s="35"/>
+    <row r="175" spans="1:26" ht="30.75" thickBot="1">
+      <c r="A175" s="24"/>
       <c r="B175" s="7" t="s">
         <v>181</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D175" s="6"/>
+      <c r="D175" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E175" s="5"/>
       <c r="F175" s="5"/>
       <c r="G175" s="5"/>
@@ -32383,16 +32713,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="A149:A157"/>
-    <mergeCell ref="A158:A165"/>
-    <mergeCell ref="A166:A175"/>
-    <mergeCell ref="A132:C132"/>
-    <mergeCell ref="A133:A137"/>
-    <mergeCell ref="A138:C138"/>
-    <mergeCell ref="A139:A141"/>
-    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:A38"/>
     <mergeCell ref="A143:A144"/>
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="A47:C47"/>
@@ -32400,12 +32726,16 @@
     <mergeCell ref="A53:A69"/>
     <mergeCell ref="A70:A76"/>
     <mergeCell ref="A77:A131"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A132:C132"/>
+    <mergeCell ref="A133:A137"/>
+    <mergeCell ref="A138:C138"/>
+    <mergeCell ref="A139:A141"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="A149:A157"/>
+    <mergeCell ref="A158:A165"/>
+    <mergeCell ref="A166:A175"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>